<commit_message>
password input modified - password character is now an asterisk
</commit_message>
<xml_diff>
--- a/MobiStore/Data/Reports/Output/Excel/reports-out.xlsx
+++ b/MobiStore/Data/Reports/Output/Excel/reports-out.xlsx
@@ -5,9 +5,9 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="MobiStore Banishora - Sofia" sheetId="37" r:id="rId38"/>
-    <sheet name="MobiStore Dragoman - Sofia" sheetId="38" r:id="rId39"/>
-    <sheet name="MobiStore Mladost - Sofia" sheetId="39" r:id="rId40"/>
+    <sheet name="MobiStore Banishora - Sofia" sheetId="40" r:id="rId41"/>
+    <sheet name="MobiStore Dragoman - Sofia" sheetId="41" r:id="rId42"/>
+    <sheet name="MobiStore Mladost - Sofia" sheetId="42" r:id="rId43"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -124,7 +124,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D605"/>
   <sheetViews>
@@ -8613,7 +8613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D605"/>
   <sheetViews>
@@ -17102,7 +17102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D806"/>
   <sheetViews>

</xml_diff>